<commit_message>
excel reader and setup class
</commit_message>
<xml_diff>
--- a/src/main/resources/setup/initialSetup.xlsx
+++ b/src/main/resources/setup/initialSetup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
@@ -17,25 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>apellido</t>
-  </si>
-  <si>
-    <t>caso</t>
-  </si>
-  <si>
-    <t>rodrigo</t>
-  </si>
-  <si>
-    <t>huanca</t>
-  </si>
-  <si>
-    <t>torrez</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>firstName</t>
   </si>
@@ -43,9 +25,6 @@
     <t>LastName</t>
   </si>
   <si>
-    <t xml:space="preserve">JhordanAPI-Contact </t>
-  </si>
-  <si>
     <t>SotoAPI-Contact</t>
   </si>
   <si>
@@ -80,13 +59,37 @@
   </si>
   <si>
     <t>Qualification</t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Working</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Campaing created by API</t>
+  </si>
+  <si>
+    <t>JhordanAPI-Contact</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +100,12 @@
     <font>
       <sz val="9"/>
       <color rgb="FF0451A5"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFA31515"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -121,10 +130,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -428,58 +440,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -489,11 +493,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -507,29 +509,31 @@
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
         <v>300</v>
       </c>
     </row>
@@ -541,74 +545,66 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>